<commit_message>
fixed kml writer and algorithm for ring distances
</commit_message>
<xml_diff>
--- a/fixtures/output/01043110000366247_acute_bkdn.xlsx
+++ b/fixtures/output/01043110000366247_acute_bkdn.xlsx
@@ -433,7 +433,7 @@
         <v>9</v>
       </c>
       <c r="F2" t="n">
-        <v>0.671894620274</v>
+        <v>0.6544732734249999</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -456,7 +456,7 @@
         <v>9</v>
       </c>
       <c r="F3" t="n">
-        <v>0.570476564384</v>
+        <v>0.555684854795</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -479,7 +479,7 @@
         <v>9</v>
       </c>
       <c r="F4" t="n">
-        <v>19.7258118707</v>
+        <v>19.2143474236</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Enable unittest to work with revised allinner and allouter
</commit_message>
<xml_diff>
--- a/fixtures/output/01043110000366247_acute_bkdn.xlsx
+++ b/fixtures/output/01043110000366247_acute_bkdn.xlsx
@@ -57,10 +57,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -86,8 +94,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -394,25 +403,25 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
User supplied receptors are now included in the outputs
</commit_message>
<xml_diff>
--- a/fixtures/output/01043110000366247_acute_bkdn.xlsx
+++ b/fixtures/output/01043110000366247_acute_bkdn.xlsx
@@ -394,7 +394,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,13 +436,13 @@
         <v/>
       </c>
       <c r="D2" t="n">
-        <v>0.390476381918</v>
+        <v>0.390602623562</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6544732734249999</v>
+        <v>0.398685747945</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -450,7 +450,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -459,13 +459,13 @@
         <v/>
       </c>
       <c r="D3" t="n">
-        <v>0.331536550685</v>
+        <v>0.390602623562</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
       </c>
       <c r="F3" t="n">
-        <v>0.555684854795</v>
+        <v>0.398685747945</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -473,24 +473,231 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="n">
+        <v/>
+      </c>
+      <c r="D4" t="n">
+        <v>0.390602623562</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.398685747945</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="n">
+        <v/>
+      </c>
+      <c r="D5" t="n">
+        <v>0.390602623562</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.398685747945</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="n">
+        <v/>
+      </c>
+      <c r="D6" t="n">
+        <v>0.331643736986</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.338506767123</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="n">
+        <v/>
+      </c>
+      <c r="D7" t="n">
+        <v>0.331643736986</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.338506767123</v>
+      </c>
+      <c r="G7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="n">
+        <v/>
+      </c>
+      <c r="D8" t="n">
+        <v>0.331643736986</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.338506767123</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="n">
+        <v/>
+      </c>
+      <c r="D9" t="n">
+        <v>0.331643736986</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.338506767123</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="n">
-        <v/>
-      </c>
-      <c r="D4" t="n">
-        <v>11.4637971748</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="n">
-        <v>19.2143474236</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
+        <v/>
+      </c>
+      <c r="D10" t="n">
+        <v>11.4675034389</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="n">
+        <v>11.7048117699</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="n">
+        <v/>
+      </c>
+      <c r="D11" t="n">
+        <v>11.4675034389</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="n">
+        <v>11.7048117699</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="n">
+        <v/>
+      </c>
+      <c r="D12" t="n">
+        <v>11.4675034389</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="n">
+        <v>11.7048117699</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="n">
+        <v/>
+      </c>
+      <c r="D13" t="n">
+        <v>11.4675034389</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="n">
+        <v>11.7048117699</v>
+      </c>
+      <c r="G13" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrected alternate receptor use and plotfile name for dep
</commit_message>
<xml_diff>
--- a/fixtures/output/01043110000366247_acute_bkdn.xlsx
+++ b/fixtures/output/01043110000366247_acute_bkdn.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Pollutant</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>CEOT0001</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
   <si>
     <t>N</t>
@@ -432,66 +435,66 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="n">
-        <v/>
+      <c r="C2" t="s">
+        <v>9</v>
       </c>
       <c r="D2" t="n">
         <v>0.390602623562</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" t="n">
         <v>0.654533649863</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="n">
-        <v/>
+      <c r="C3" t="s">
+        <v>9</v>
       </c>
       <c r="D3" t="n">
         <v>0.331643736986</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" t="n">
         <v>0.555736117808</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="n">
-        <v/>
+      <c r="C4" t="s">
+        <v>9</v>
       </c>
       <c r="D4" t="n">
         <v>11.4675034389</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" t="n">
         <v>19.2161199847</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected max offsite impacts module for discrete receptors
</commit_message>
<xml_diff>
--- a/fixtures/output/01043110000366247_acute_bkdn.xlsx
+++ b/fixtures/output/01043110000366247_acute_bkdn.xlsx
@@ -25,13 +25,13 @@
     <t>Emission type</t>
   </si>
   <si>
-    <t>Max conc at populated receptor (µg/m3)</t>
+    <t>Max conc at populated receptor (ug/m3)</t>
   </si>
   <si>
     <t>Is max populated receptor interpolated? (Y/N)</t>
   </si>
   <si>
-    <t>Max conc at any receptor (µg/m3)</t>
+    <t>Max conc at any receptor (ug/m3)</t>
   </si>
   <si>
     <t>Is max conc at any receptor interpolated? (Y/N)</t>

</xml_diff>